<commit_message>
Update Excel Reading We solve the issue with the 'nan' in the pandas when reading from excel. We solve it by removing the 'nan' from the vector being passed by including  mt=mt[~pd.isnull(mt)] in the mortality_table.py.
</commit_message>
<xml_diff>
--- a/soa_tables/tables_manual.xlsx
+++ b/soa_tables/tables_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrocortereal/Dropbox (MagentaKoncept)/PedroCR/PycharmProjects/lifeActuary/soa_tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC40A0D-93F4-3A4A-B1D6-FAB2B34F4916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C6545D-0AD5-421E-AE27-D2CB150FD8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16620" activeTab="1" xr2:uid="{BD97DD2D-0F63-8D44-8A57-7FC915C77CD0}"/>
+    <workbookView xWindow="5153" yWindow="1013" windowWidth="16875" windowHeight="10432" activeTab="1" xr2:uid="{BD97DD2D-0F63-8D44-8A57-7FC915C77CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="qx" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>TV7377</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>GRM95</t>
+  </si>
+  <si>
+    <t>S2PMA</t>
+  </si>
+  <si>
+    <t>S2PFA</t>
   </si>
 </sst>
 </file>
@@ -101,9 +107,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -141,7 +147,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -247,7 +253,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -400,12 +406,12 @@
   <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -427,7 +433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1.1679999999999999E-2</v>
       </c>
@@ -438,7 +444,7 @@
         <v>1.2879E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>9.7134529999999997E-4</v>
       </c>
@@ -449,7 +455,7 @@
         <v>1.289E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>5.9755310000000005E-4</v>
       </c>
@@ -460,7 +466,7 @@
         <v>1.2902E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>4.661674E-4</v>
       </c>
@@ -471,7 +477,7 @@
         <v>1.2913E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>3.8527439999999999E-4</v>
       </c>
@@ -482,7 +488,7 @@
         <v>1.2924E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>3.4485210000000002E-4</v>
       </c>
@@ -493,7 +499,7 @@
         <v>1.2936E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>3.1453239999999999E-4</v>
       </c>
@@ -504,7 +510,7 @@
         <v>1.2947E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>2.943326E-4</v>
       </c>
@@ -515,7 +521,7 @@
         <v>1.2957999999999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>2.7411450000000001E-4</v>
       </c>
@@ -526,7 +532,7 @@
         <v>1.297E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>2.5387929999999998E-4</v>
       </c>
@@ -537,7 +543,7 @@
         <v>1.2980999999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>2.3362820000000001E-4</v>
       </c>
@@ -548,7 +554,7 @@
         <v>1.2991999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>2.336828E-4</v>
       </c>
@@ -559,7 +565,7 @@
         <v>1.3004E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>2.23575E-4</v>
       </c>
@@ -570,7 +576,7 @@
         <v>1.3014999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>2.5411930000000002E-4</v>
       </c>
@@ -581,7 +587,7 @@
         <v>1.3025999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>3.0502060000000002E-4</v>
       </c>
@@ -592,7 +598,7 @@
         <v>1.3037999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>3.8647740000000001E-4</v>
       </c>
@@ -603,7 +609,7 @@
         <v>1.3056999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>4.7819630000000001E-4</v>
       </c>
@@ -614,7 +620,7 @@
         <v>1.3146E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>5.8021760000000005E-4</v>
       </c>
@@ -625,7 +631,7 @@
         <v>1.3324999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>6.4166549999999998E-4</v>
       </c>
@@ -636,7 +642,7 @@
         <v>1.3596000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>6.5226919999999999E-4</v>
       </c>
@@ -647,7 +653,7 @@
         <v>1.3965E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>6.3229819999999996E-4</v>
       </c>
@@ -658,7 +664,7 @@
         <v>1.4436E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>6.2249340000000003E-4</v>
       </c>
@@ -669,7 +675,7 @@
         <v>1.5014E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>6.024588E-4</v>
       </c>
@@ -680,7 +686,7 @@
         <v>1.5709999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>5.9260469999999996E-4</v>
       </c>
@@ -691,7 +697,7 @@
         <v>1.6535E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>6.1340289999999996E-4</v>
       </c>
@@ -702,7 +708,7 @@
         <v>1.7501000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>6.0354970000000001E-4</v>
       </c>
@@ -713,7 +719,7 @@
         <v>1.8617E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>6.1415000000000005E-4</v>
       </c>
@@ -724,7 +730,7 @@
         <v>1.9895999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>6.2476960000000005E-4</v>
       </c>
@@ -735,7 +741,7 @@
         <v>2.1348000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>6.7640280000000005E-4</v>
       </c>
@@ -746,7 +752,7 @@
         <v>2.2989999999999998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>7.1788250000000004E-4</v>
       </c>
@@ -757,7 +763,7 @@
         <v>2.4854999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>7.389238E-4</v>
       </c>
@@ -768,7 +774,7 @@
         <v>2.6984000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>7.9082239999999997E-4</v>
       </c>
@@ -779,7 +785,7 @@
         <v>2.9413999999999998E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>8.4284099999999999E-4</v>
       </c>
@@ -790,7 +796,7 @@
         <v>3.2187000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>9.0527529999999998E-4</v>
       </c>
@@ -801,7 +807,7 @@
         <v>3.5338000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>9.781713E-4</v>
       </c>
@@ -812,7 +818,7 @@
         <v>3.8714999999999999E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>1.0615821E-3</v>
       </c>
@@ -823,7 +829,7 @@
         <v>4.2176000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>1.1349331999999999E-3</v>
       </c>
@@ -834,7 +840,7 @@
         <v>4.5777999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>1.2498450999999999E-3</v>
       </c>
@@ -845,7 +851,7 @@
         <v>4.9576000000000004E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>1.3444891E-3</v>
       </c>
@@ -856,7 +862,7 @@
         <v>5.3626000000000004E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>1.470573E-3</v>
       </c>
@@ -867,7 +873,7 @@
         <v>5.7984999999999998E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>1.6179384000000001E-3</v>
       </c>
@@ -878,7 +884,7 @@
         <v>6.2708E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>1.755607E-3</v>
       </c>
@@ -889,7 +895,7 @@
         <v>6.7850999999999996E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>1.9147917999999999E-3</v>
       </c>
@@ -900,7 +906,7 @@
         <v>7.3470000000000002E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>2.1165676E-3</v>
       </c>
@@ -911,7 +917,7 @@
         <v>7.9620999999999997E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>2.3195796000000002E-3</v>
       </c>
@@ -922,7 +928,7 @@
         <v>8.6361000000000007E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>2.5134837999999998E-3</v>
       </c>
@@ -933,7 +939,7 @@
         <v>9.3743999999999997E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>2.7508006000000001E-3</v>
       </c>
@@ -944,7 +950,7 @@
         <v>1.0182800000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>3.0005369000000001E-3</v>
       </c>
@@ -955,7 +961,7 @@
         <v>1.10668E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>3.2735644000000002E-3</v>
       </c>
@@ -966,7 +972,7 @@
         <v>1.19579E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>3.5173963E-3</v>
       </c>
@@ -977,7 +983,7 @@
         <v>1.2818100000000001E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>3.7637152E-3</v>
       </c>
@@ -988,7 +994,7 @@
         <v>1.3696699999999999E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>4.0554097000000001E-3</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>1.464E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>4.4148217999999996E-3</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>1.5691299999999998E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>4.7895812999999999E-3</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>1.6891199999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>5.1695235999999999E-3</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>1.8277600000000001E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>5.5333906000000002E-3</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>1.98861E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>5.9030586999999999E-3</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>2.1749600000000001E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>6.3119928E-3</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>2.3889199999999999E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>6.7504758999999996E-3</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>2.6286299999999999E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>7.2197338999999998E-3</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>2.8913899999999999E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>7.7323636999999997E-3</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>3.1746200000000002E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>8.4033613000000004E-3</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>3.4758699999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>9.2615826999999998E-3</v>
       </c>
@@ -1120,7 +1126,7 @@
         <v>3.7927900000000001E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>1.0188575E-2</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>4.12316E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>1.11890389E-2</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>4.4648500000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>1.2338999E-2</v>
       </c>
@@ -1153,7 +1159,7 @@
         <v>4.8158699999999999E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>1.36722007E-2</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>5.1742999999999997E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>1.51778599E-2</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>5.5383300000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>1.6919851400000002E-2</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>5.9062400000000001E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>1.89820531E-2</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>6.2764200000000006E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>2.1319874400000001E-2</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>6.6473199999999996E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>2.3940661500000002E-2</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>7.0175000000000001E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>2.6870200600000001E-2</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>7.3892399999999997E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>3.0169584199999998E-2</v>
       </c>
@@ -1241,7 +1247,7 @@
         <v>7.7790700000000004E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>3.4013029899999998E-2</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>8.2060300000000003E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>3.8568217000000002E-2</v>
       </c>
@@ -1263,7 +1269,7 @@
         <v>8.6879999999999999E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>4.3713938700000003E-2</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>9.2416600000000002E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>4.9443483000000003E-2</v>
       </c>
@@ -1285,7 +1291,7 @@
         <v>9.8826300000000006E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>5.5840446299999999E-2</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>0.1062543</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>6.2805180099999997E-2</v>
       </c>
@@ -1307,7 +1313,7 @@
         <v>0.1145014</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>7.0374145799999996E-2</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>0.1232765</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>7.8849043600000002E-2</v>
       </c>
@@ -1329,7 +1335,7 @@
         <v>0.13257939999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>8.8442122400000003E-2</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>0.14241019999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>9.9030253200000001E-2</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>0.15276899999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>0.1099420228</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>0.16365560000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>0.1213510253</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>0.17507020000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>0.13409527730000001</v>
       </c>
@@ -1384,7 +1390,7 @@
         <v>0.1870127</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>0.14816282850000001</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>0.19948299999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>0.16341724439999999</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>0.21248130000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>0.17998776350000001</v>
       </c>
@@ -1417,7 +1423,7 @@
         <v>0.2260075</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>0.19609306109999999</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>0.24006150000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>0.21009112390000001</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>0.25464350000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A95">
         <v>0.22238837859999999</v>
       </c>
@@ -1450,7 +1456,7 @@
         <v>0.26975339999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A96">
         <v>0.23475274730000001</v>
       </c>
@@ -1461,7 +1467,7 @@
         <v>0.28539120000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A97">
         <v>0.24789086339999999</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>0.30155690000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A98">
         <v>0.26205250600000002</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>0.31825039999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A99">
         <v>0.27619663649999998</v>
       </c>
@@ -1494,7 +1500,7 @@
         <v>0.33547189999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A100">
         <v>0.29177837350000002</v>
       </c>
@@ -1505,7 +1511,7 @@
         <v>0.35322130000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A101">
         <v>0.30725552049999999</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>0.37149860000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A102">
         <v>0.51639344259999997</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>0.39030379999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A103">
         <v>0.55367231640000003</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>0.40963699999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A104">
         <v>0.59071729959999997</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>0.42949799999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A105">
         <v>0.6288659794</v>
       </c>
@@ -1560,7 +1566,7 @@
         <v>0.44988689999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A106">
         <v>0.66666666669999997</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>0.47080369999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A107">
         <v>0.66666666669999997</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>0.49224839999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A108">
         <v>0.75</v>
       </c>
@@ -1593,7 +1599,7 @@
         <v>0.51422109999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A109">
         <v>1</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>0.53672160000000002</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B110">
         <v>0.47082459999999998</v>
       </c>
@@ -1612,7 +1618,7 @@
         <v>0.55974999999999997</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B111">
         <v>0.49339889999999997</v>
       </c>
@@ -1620,7 +1626,7 @@
         <v>0.5833064</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B112">
         <v>0.51655949999999995</v>
       </c>
@@ -1628,7 +1634,7 @@
         <v>0.6073906</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B113">
         <v>0.54030650000000002</v>
       </c>
@@ -1636,7 +1642,7 @@
         <v>0.63200279999999998</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B114">
         <v>1</v>
       </c>
@@ -1651,15 +1657,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3D354C-BD1A-3C40-811D-4A63139399CE}">
-  <dimension ref="A1:D130"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1669,8 +1675,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1680,8 +1692,14 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>100000</v>
       </c>
@@ -1691,9 +1709,14 @@
       <c r="C3" s="1">
         <v>100000</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>98832</v>
       </c>
@@ -1703,9 +1726,14 @@
       <c r="C4" s="1">
         <v>100000</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>98736.0000013104</v>
       </c>
@@ -1715,9 +1743,14 @@
       <c r="C5" s="1">
         <v>100000</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>98676.999998428</v>
       </c>
@@ -1727,9 +1760,14 @@
       <c r="C6" s="1">
         <v>100000</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E6">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>98630.999997898907</v>
       </c>
@@ -1739,9 +1777,14 @@
       <c r="C7" s="1">
         <v>100000</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E7">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>98592.999998553307</v>
       </c>
@@ -1751,9 +1794,14 @@
       <c r="C8" s="1">
         <v>100000</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>98558.999995458493</v>
       </c>
@@ -1763,9 +1811,14 @@
       <c r="C9" s="1">
         <v>100000</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E9">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>98527.999996648301</v>
       </c>
@@ -1775,9 +1828,14 @@
       <c r="C10" s="1">
         <v>100000</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E10">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>98498.999994236496</v>
       </c>
@@ -1787,9 +1845,14 @@
       <c r="C11" s="1">
         <v>100000</v>
       </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E11">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>98471.999990102602</v>
       </c>
@@ -1799,9 +1862,14 @@
       <c r="C12" s="1">
         <v>100000</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E12">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>98446.999987675503</v>
       </c>
@@ -1811,9 +1879,14 @@
       <c r="C13" s="1">
         <v>100000</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E13">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>98423.999992273006</v>
       </c>
@@ -1823,9 +1896,14 @@
       <c r="C14" s="1">
         <v>100000</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E14">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>98400.999996367595</v>
       </c>
@@ -1835,9 +1913,14 @@
       <c r="C15" s="1">
         <v>100000</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E15">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>98378.999992793397</v>
       </c>
@@ -1847,9 +1930,14 @@
       <c r="C16" s="1">
         <v>100000</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E16">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>98353.999990180499</v>
       </c>
@@ -1859,9 +1947,14 @@
       <c r="C17" s="1">
         <v>100000</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E17">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>98323.999994091093</v>
       </c>
@@ -1871,9 +1964,14 @@
       <c r="C18" s="1">
         <v>100000</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E18">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>98285.999990215802</v>
       </c>
@@ -1883,9 +1981,14 @@
       <c r="C19" s="1">
         <v>99871.21</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E19">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>98238.999988678697</v>
       </c>
@@ -1895,9 +1998,14 @@
       <c r="C20" s="1">
         <v>99742.476010309998</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <v>999697</v>
+      </c>
+      <c r="E20">
+        <v>999829</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>98181.999991878896</v>
       </c>
@@ -1907,9 +2015,14 @@
       <c r="C21" s="1">
         <v>99613.788267761498</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="1">
+        <v>999387.09</v>
+      </c>
+      <c r="E21">
+        <v>999654.03</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>98118.999989763106</v>
       </c>
@@ -1919,9 +2032,14 @@
       <c r="C22" s="1">
         <v>99485.156982971297</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="1">
+        <v>999069.29</v>
+      </c>
+      <c r="E22">
+        <v>999473.09</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>98054.999988134907</v>
       </c>
@@ -1931,9 +2049,14 @@
       <c r="C23" s="1">
         <v>99356.582366086499</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="1">
+        <v>998742.59</v>
+      </c>
+      <c r="E23">
+        <v>999286.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>97992.999988141397</v>
       </c>
@@ -1943,9 +2066,14 @@
       <c r="C24" s="1">
         <v>99228.054691137804</v>
       </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="1">
+        <v>998407.02</v>
+      </c>
+      <c r="E24">
+        <v>999092.33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>97931.999992402605</v>
       </c>
@@ -1955,9 +2083,14 @@
       <c r="C25" s="1">
         <v>99099.584128729097</v>
       </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="1">
+        <v>998060.57</v>
+      </c>
+      <c r="E25">
+        <v>998889.51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>97872.999997205596</v>
       </c>
@@ -1967,9 +2100,14 @@
       <c r="C26" s="1">
         <v>98971.170887615095</v>
       </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="1">
+        <v>997702.26</v>
+      </c>
+      <c r="E26">
+        <v>998676.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>97814.9999974042</v>
       </c>
@@ -1979,9 +2117,14 @@
       <c r="C27" s="1">
         <v>98842.805278973901</v>
       </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="1">
+        <v>997329.12</v>
+      </c>
+      <c r="E27">
+        <v>998451.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>97754.999992742203</v>
       </c>
@@ -1991,9 +2134,14 @@
       <c r="C28" s="1">
         <v>98714.497433441298</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="1">
+        <v>996941.16</v>
+      </c>
+      <c r="E28">
+        <v>998211.42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>97695.999991823104</v>
       </c>
@@ -2003,9 +2151,14 @@
       <c r="C29" s="1">
         <v>98586.247558375704</v>
       </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="1">
+        <v>996535.41</v>
+      </c>
+      <c r="E29">
+        <v>997955.88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>97635.999993428195</v>
       </c>
@@ -2015,8 +2168,14 @@
       <c r="C30">
         <v>98458.046002050804</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>996109.89</v>
+      </c>
+      <c r="E30">
+        <v>997680.44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>97574.999988766605</v>
       </c>
@@ -2026,8 +2185,14 @@
       <c r="C31">
         <v>98329.9028551792</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>995663.63</v>
+      </c>
+      <c r="E31">
+        <v>997383.13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>97508.999985564195</v>
       </c>
@@ -2037,8 +2202,14 @@
       <c r="C32">
         <v>98201.818323719999</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>995192.68</v>
+      </c>
+      <c r="E32">
+        <v>997060.98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>97438.999980882101</v>
       </c>
@@ -2048,8 +2219,14 @@
       <c r="C33">
         <v>98073.782792989601</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>994695.08</v>
+      </c>
+      <c r="E33">
+        <v>996710.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>97366.999984748007</v>
       </c>
@@ -2059,8 +2236,14 @@
       <c r="C34">
         <v>97945.727854796802</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>994167.9</v>
+      </c>
+      <c r="E34">
+        <v>996326.28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>97289.999980139299</v>
       </c>
@@ -2070,8 +2253,14 @@
       <c r="C35">
         <v>97816.968400958795</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>993608.18</v>
+      </c>
+      <c r="E35">
+        <v>995904.83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>97207.999979265995</v>
       </c>
@@ -2081,8 +2270,14 @@
       <c r="C36">
         <v>97686.627290564604</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>993011.02</v>
+      </c>
+      <c r="E36">
+        <v>995440.74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>97119.999977922402</v>
       </c>
@@ -2092,8 +2287,14 @@
       <c r="C37">
         <v>97553.812552100295</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>992373.51</v>
+      </c>
+      <c r="E37">
+        <v>994929.09</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>97024.999981287998</v>
       </c>
@@ -2103,8 +2304,14 @@
       <c r="C38">
         <v>97417.578652871307</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>991690.76</v>
+      </c>
+      <c r="E38">
+        <v>994363.97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>96921.999978055406</v>
       </c>
@@ -2114,8 +2321,14 @@
       <c r="C39">
         <v>97276.946636327993</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>990957.9</v>
+      </c>
+      <c r="E39">
+        <v>993738.51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>96811.999982469904</v>
       </c>
@@ -2125,8 +2338,14 @@
       <c r="C40">
         <v>97130.8950286482</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>990170.08</v>
+      </c>
+      <c r="E40">
+        <v>993046.87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>96690.999978670603</v>
       </c>
@@ -2136,8 +2355,14 @@
       <c r="C41">
         <v>96978.302392558195</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>989321.51</v>
+      </c>
+      <c r="E41">
+        <v>992281.23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>96560.999983131202</v>
       </c>
@@ -2147,8 +2372,14 @@
       <c r="C42">
         <v>96817.948769552095</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>988406.39</v>
+      </c>
+      <c r="E42">
+        <v>991433.82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>96418.999983703005</v>
       </c>
@@ -2158,8 +2389,14 @@
       <c r="C43">
         <v>96648.507677410598</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>987417.98</v>
+      </c>
+      <c r="E43">
+        <v>990495.93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>96262.999981139699</v>
       </c>
@@ -2169,8 +2406,14 @@
       <c r="C44">
         <v>96468.577150667494</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>986348.61</v>
+      </c>
+      <c r="E44">
+        <v>989459.87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>96093.999984531896</v>
       </c>
@@ -2180,8 +2423,14 @@
       <c r="C45">
         <v>96276.643269568594</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>985191.62</v>
+      </c>
+      <c r="E45">
+        <v>988316.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>95909.999981332294</v>
       </c>
@@ -2191,8 +2440,14 @@
       <c r="C46">
         <v>96071.111891516703</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>983937.47</v>
+      </c>
+      <c r="E46">
+        <v>987055.95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>95706.999982855807</v>
       </c>
@@ -2202,8 +2457,14 @@
       <c r="C47">
         <v>95850.244405278107</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>982576.68</v>
+      </c>
+      <c r="E47">
+        <v>985670.12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>95484.999978118401</v>
       </c>
@@ -2213,8 +2474,14 @@
       <c r="C48">
         <v>95612.008622808804</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>981100.85</v>
+      </c>
+      <c r="E48">
+        <v>984148.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>95244.999977530402</v>
       </c>
@@ -2224,8 +2491,14 @@
       <c r="C49">
         <v>95354.009178741006</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>979498.72</v>
+      </c>
+      <c r="E49">
+        <v>982482.08</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>94982.999974445207</v>
       </c>
@@ -2235,8 +2508,14 @@
       <c r="C50">
         <v>95073.534896142606</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>977758.15</v>
+      </c>
+      <c r="E50">
+        <v>980660.56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>94697.999978149106</v>
       </c>
@@ -2246,8 +2525,14 @@
       <c r="C51">
         <v>94767.521709372406</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>975868.14</v>
+      </c>
+      <c r="E51">
+        <v>978674.73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>94387.999976669496</v>
       </c>
@@ -2257,8 +2542,14 @@
       <c r="C52">
         <v>94432.632241155807</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>973815.89</v>
+      </c>
+      <c r="E52">
+        <v>976515.77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>94055.999974787104</v>
       </c>
@@ -2268,8 +2559,14 @@
       <c r="C53">
         <v>94067.036305434201</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>971585.85</v>
+      </c>
+      <c r="E53">
+        <v>974173.11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>93701.999978030799</v>
       </c>
@@ -2279,8 +2576,14 @@
       <c r="C54">
         <v>93670.299173112406</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>969162.72</v>
+      </c>
+      <c r="E54">
+        <v>971639.28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>93321.999978410502</v>
       </c>
@@ -2290,8 +2593,14 @@
       <c r="C55">
         <v>93241.495277557697</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>966529.5</v>
+      </c>
+      <c r="E55">
+        <v>968906.06</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>92909.999978486201</v>
       </c>
@@ -2301,8 +2610,14 @@
       <c r="C56">
         <v>92779.241240569696</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>963668.57</v>
+      </c>
+      <c r="E56">
+        <v>965967.37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>92464.999980006294</v>
       </c>
@@ -2312,8 +2627,14 @@
       <c r="C57">
         <v>92281.703281492999</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>960560.74</v>
+      </c>
+      <c r="E57">
+        <v>962816.38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>91986.999980435605</v>
       </c>
@@ -2323,8 +2644,14 @@
       <c r="C58">
         <v>91746.607825015293</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>957187.25</v>
+      </c>
+      <c r="E58">
+        <v>959449.42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>91477.9999794217</v>
       </c>
@@ -2334,8 +2661,14 @@
       <c r="C59">
         <v>91171.283196666205</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>953527.93</v>
+      </c>
+      <c r="E59">
+        <v>955862.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>90937.999975784594</v>
       </c>
@@ -2345,8 +2678,14 @@
       <c r="C60">
         <v>90552.676923048493</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>949562.2</v>
+      </c>
+      <c r="E60">
+        <v>952053.88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>90363.999974691003</v>
       </c>
@@ -2356,8 +2695,14 @@
       <c r="C61">
         <v>89887.386405694895</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>945267.33</v>
+      </c>
+      <c r="E61">
+        <v>948023.84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>89753.999970634293</v>
       </c>
@@ -2367,8 +2712,14 @@
       <c r="C62">
         <v>89171.694046394099</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>940621.35</v>
+      </c>
+      <c r="E62">
+        <v>943772.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>89105.999974385704</v>
       </c>
@@ -2378,8 +2729,14 @@
       <c r="C63">
         <v>88401.598379439994</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>935600.31</v>
+      </c>
+      <c r="E63">
+        <v>939304.13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>88416.999974731501</v>
       </c>
@@ -2389,8 +2746,14 @@
       <c r="C64">
         <v>87572.886435591805</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>930176.63</v>
+      </c>
+      <c r="E64">
+        <v>934616.07</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>87673.999978881795</v>
       </c>
@@ -2400,8 +2763,14 @@
       <c r="C65">
         <v>86681.1492475954</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>924296.99</v>
+      </c>
+      <c r="E65">
+        <v>929675.68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>86861.999977437605</v>
       </c>
@@ -2411,8 +2780,14 @@
       <c r="C66">
         <v>85721.866305102099</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>917896.23</v>
+      </c>
+      <c r="E66">
+        <v>924436.96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>85976.999976017396</v>
       </c>
@@ -2422,8 +2797,14 @@
       <c r="C67">
         <v>84696.812800012398</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>910900.03</v>
+      </c>
+      <c r="E67">
+        <v>918846.89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>85014.999978780499</v>
       </c>
@@ -2433,8 +2814,14 @@
       <c r="C68">
         <v>83611.160583860503</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>903226.6</v>
+      </c>
+      <c r="E68">
+        <v>912845.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>83965.999979057306</v>
       </c>
@@ -2444,8 +2831,14 @@
       <c r="C69">
         <v>82465.963600691597</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>894786.85</v>
+      </c>
+      <c r="E69">
+        <v>906364.7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>82817.999975367406</v>
       </c>
@@ -2455,8 +2848,14 @@
       <c r="C70">
         <v>81258.661893577402</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>885485.55</v>
+      </c>
+      <c r="E70">
+        <v>899327.68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>81560.999974543098</v>
       </c>
@@ -2466,8 +2865,14 @@
       <c r="C71">
         <v>79983.607852206798</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>875220.11</v>
+      </c>
+      <c r="E71">
+        <v>891646.52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>80180.999974938401</v>
       </c>
@@ -2477,8 +2882,14 @@
       <c r="C72">
         <v>78632.588735253594</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>863879.01</v>
+      </c>
+      <c r="E72">
+        <v>883224.03</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>78658.999975803104</v>
       </c>
@@ -2488,8 +2899,14 @@
       <c r="C73">
         <v>77195.373731386106</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>851343.26</v>
+      </c>
+      <c r="E73">
+        <v>873952.83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>76981.999975889295</v>
       </c>
@@ -2499,8 +2916,14 @@
       <c r="C74">
         <v>75660.258809826395</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>837485.95</v>
+      </c>
+      <c r="E74">
+        <v>863714.47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>75138.9999728736</v>
       </c>
@@ -2510,8 +2933,14 @@
       <c r="C75">
         <v>74014.678444816207</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>822174.19</v>
+      </c>
+      <c r="E75">
+        <v>852380.81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>73119.999970719</v>
       </c>
@@ -2521,8 +2950,14 @@
       <c r="C76">
         <v>72246.526988512298</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>805272.76</v>
+      </c>
+      <c r="E76">
+        <v>839812.45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>70913.999974898397</v>
       </c>
@@ -2532,8 +2967,14 @@
       <c r="C77">
         <v>70347.433106134107</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>786644.38</v>
+      </c>
+      <c r="E77">
+        <v>825860.65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>68501.999973423604</v>
       </c>
@@ -2543,8 +2984,14 @@
       <c r="C78">
         <v>68313.414460046697</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>766155.44</v>
+      </c>
+      <c r="E78">
+        <v>810365.85</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>65859.999973514598</v>
       </c>
@@ -2554,8 +3001,14 @@
       <c r="C79">
         <v>66144.723141915194</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>743681.04</v>
+      </c>
+      <c r="E79">
+        <v>793164.22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>62980.9999718904</v>
       </c>
@@ -2565,8 +3018,14 @@
       <c r="C80">
         <v>63845.6185536423</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>719108.33</v>
+      </c>
+      <c r="E80">
+        <v>774091</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>59866.999970457196</v>
       </c>
@@ -2576,8 +3035,14 @@
       <c r="C81">
         <v>61424.0883177016</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>692346.71</v>
+      </c>
+      <c r="E81">
+        <v>752986.18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>56523.999973464801</v>
       </c>
@@ -2587,8 +3052,14 @@
       <c r="C82">
         <v>58891.474877821398</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>663331.85</v>
+      </c>
+      <c r="E82">
+        <v>729698.58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>52973.999975158898</v>
       </c>
@@ -2598,8 +3069,14 @@
       <c r="C83">
         <v>56262.058861739002</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>632036.51</v>
+      </c>
+      <c r="E83">
+        <v>704094.18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>49245.999977297899</v>
       </c>
@@ -2609,8 +3086,14 @@
       <c r="C84">
         <v>53552.551247634197</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>598486.12</v>
+      </c>
+      <c r="E84">
+        <v>676069.12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>45362.999977962303</v>
       </c>
@@ -2620,8 +3103,14 @@
       <c r="C85">
         <v>50781.581588427798</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>562770.86</v>
+      </c>
+      <c r="E85">
+        <v>645562.18000000005</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>41350.999981480199</v>
       </c>
@@ -2631,8 +3120,14 @@
       <c r="C86">
         <v>47969.130020841498</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>525052.82999999996</v>
+      </c>
+      <c r="E86">
+        <v>612568.79</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>37255.999983241003</v>
       </c>
@@ -2642,8 +3137,14 @@
       <c r="C87">
         <v>45135.958075898503</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>485571.49</v>
+      </c>
+      <c r="E87">
+        <v>577151.28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>33159.999983646703</v>
       </c>
@@ -2653,8 +3154,14 @@
       <c r="C88">
         <v>42303.035776031204</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>444649.95</v>
+      </c>
+      <c r="E88">
+        <v>539452.92000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>29135.9999866832</v>
       </c>
@@ -2664,8 +3171,14 @@
       <c r="C89">
         <v>39491.017618283899</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>402702.12</v>
+      </c>
+      <c r="E89">
+        <v>499707.64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>25228.999989056101</v>
       </c>
@@ -2675,8 +3188,14 @@
       <c r="C90">
         <v>36719.735456920796</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <v>360237.18</v>
+      </c>
+      <c r="E90">
+        <v>458247.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>21490.999990451099</v>
       </c>
@@ -2686,8 +3205,14 @@
       <c r="C91">
         <v>34006.426076643897</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <v>317847.71000000002</v>
+      </c>
+      <c r="E91">
+        <v>415508.96</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>17978.999992611101</v>
       </c>
@@ -2697,8 +3222,14 @@
       <c r="C92">
         <v>31361.042387643502</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <v>276190.59000000003</v>
+      </c>
+      <c r="E92">
+        <v>372036.75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>14742.999993974499</v>
       </c>
@@ -2708,8 +3239,14 @@
       <c r="C93">
         <v>28787.545841000701</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <v>235953.21</v>
+      </c>
+      <c r="E93">
+        <v>328471.62</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>11851.999995358799</v>
       </c>
@@ -2719,8 +3256,14 @@
       <c r="C94">
         <v>26286.483858334599</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <v>197805.95</v>
+      </c>
+      <c r="E94">
+        <v>285517.71000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A95">
         <v>9361.9999958710905</v>
       </c>
@@ -2730,8 +3273,14 @@
       <c r="C95">
         <v>23857.1763941924</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <v>162373.56</v>
+      </c>
+      <c r="E95">
+        <v>243913.78</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A96">
         <v>7279.9999963361097</v>
       </c>
@@ -2741,8 +3290,14 @@
       <c r="C96">
         <v>21499.459922706999</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <v>130203.46</v>
+      </c>
+      <c r="E96">
+        <v>204399.02</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A97">
         <v>5570.9999968522197</v>
       </c>
@@ -2752,8 +3307,14 @@
       <c r="C97">
         <v>19215.049858241699</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <v>101728.62</v>
+      </c>
+      <c r="E97">
+        <v>167674.85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A98">
         <v>4189.9999976311201</v>
       </c>
@@ -2763,8 +3324,14 @@
       <c r="C98">
         <v>17014.899748403299</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <v>77230.23</v>
+      </c>
+      <c r="E98">
+        <v>134357.19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A99">
         <v>3091.9999981118899</v>
       </c>
@@ -2774,8 +3341,14 @@
       <c r="C99">
         <v>14917.3624595692</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <v>56831.56</v>
+      </c>
+      <c r="E99">
+        <v>104934.04</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A100">
         <v>2237.9999985753798</v>
       </c>
@@ -2785,8 +3358,14 @@
       <c r="C100">
         <v>12939.627495097</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <v>40513.69</v>
+      </c>
+      <c r="E100">
+        <v>79747.88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A101">
         <v>1584.99999909805</v>
       </c>
@@ -2796,8 +3375,14 @@
       <c r="C101">
         <v>11096.892555594701</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101">
+        <v>27977.05</v>
+      </c>
+      <c r="E101">
+        <v>58893.33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A102">
         <v>1097.99999938268</v>
       </c>
@@ -2807,8 +3392,14 @@
       <c r="C102">
         <v>9401.6313767691099</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102">
+        <v>18714.66</v>
+      </c>
+      <c r="E102">
+        <v>42209.61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A103">
         <v>530.99999972666103</v>
       </c>
@@ -2818,8 +3409,14 @@
       <c r="C103">
         <v>7863.0017528251401</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103">
+        <v>12127.08</v>
+      </c>
+      <c r="E103">
+        <v>29327.11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A104">
         <v>236.999999869601</v>
       </c>
@@ -2829,8 +3426,14 @@
       <c r="C104">
         <v>6486.42446335769</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104">
+        <v>7613.04</v>
+      </c>
+      <c r="E104">
+        <v>19734.099999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A105">
         <v>96.999999941430104</v>
       </c>
@@ -2840,8 +3443,14 @@
       <c r="C105">
         <v>5273.38071111912</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <v>4630.38</v>
+      </c>
+      <c r="E105">
+        <v>12849.76</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A106">
         <v>35.999999976462703</v>
       </c>
@@ -2851,8 +3460,14 @@
       <c r="C106">
         <v>4221.4309067229397</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106">
+        <v>2728.97</v>
+      </c>
+      <c r="E106">
+        <v>8091.16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A107">
         <v>11.999999990954199</v>
       </c>
@@ -2862,8 +3477,14 @@
       <c r="C107">
         <v>3324.4557798022702</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107">
+        <v>1558.82</v>
+      </c>
+      <c r="E107">
+        <v>4924.2299999999996</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A108">
         <v>3.9999999965847501</v>
       </c>
@@ -2873,8 +3494,14 @@
       <c r="C108">
         <v>2573.1038401486098</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108">
+        <v>863.22</v>
+      </c>
+      <c r="E108">
+        <v>2895.44</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A109">
         <v>0.99999999914618698</v>
       </c>
@@ -2884,8 +3511,14 @@
       <c r="C109">
         <v>1955.4006726267701</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109">
+        <v>463.56</v>
+      </c>
+      <c r="E109">
+        <v>1644.53</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A110">
         <v>0</v>
       </c>
@@ -2895,40 +3528,70 @@
       <c r="C110">
         <v>1457.4706014467299</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110">
+        <v>241.52</v>
+      </c>
+      <c r="E110">
+        <v>902.17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B111">
         <v>5795.1718490413996</v>
       </c>
       <c r="C111">
         <v>1064.31295130643</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111">
+        <v>122.13</v>
+      </c>
+      <c r="E111">
+        <v>478.06</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B112">
         <v>4541.39105563877</v>
       </c>
       <c r="C112">
         <v>760.56740095755094</v>
       </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D112">
+        <v>59.97</v>
+      </c>
+      <c r="E112">
+        <v>244.75</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B113">
         <v>3493.6249265152801</v>
       </c>
       <c r="C113">
         <v>531.21305328373501</v>
       </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D113">
+        <v>28.61</v>
+      </c>
+      <c r="E113">
+        <v>121.11</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B114">
         <v>2635.3572704180301</v>
       </c>
       <c r="C114">
         <v>362.154286590965</v>
       </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D114">
+        <v>13.27</v>
+      </c>
+      <c r="E114">
+        <v>57.96</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B115">
         <v>1946.9885110627599</v>
       </c>
@@ -2936,7 +3599,7 @@
         <v>240.66169997514899</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B116">
         <v>1407.0307713862801</v>
       </c>
@@ -2944,7 +3607,7 @@
         <v>155.654861449717</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B117">
         <v>993.30645844632102</v>
       </c>
@@ -2952,7 +3615,7 @@
         <v>97.829298337953304</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B118">
         <v>684.05241228655996</v>
       </c>
@@ -2960,7 +3623,7 @@
         <v>59.646151445316399</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B119">
         <v>458.847514224478</v>
       </c>
@@ -2968,7 +3631,7 @@
         <v>35.212880905711302</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B120">
         <v>299.31008784774599</v>
       </c>
@@ -2976,7 +3639,7 @@
         <v>20.089018982470101</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B121">
         <v>189.53871174976101</v>
       </c>
@@ -2984,7 +3647,7 @@
         <v>11.0512325084054</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B122">
         <v>116.302735193543</v>
       </c>
@@ -2992,7 +3655,7 @@
         <v>5.8482713538878999</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B123">
         <v>69.011763530239094</v>
       </c>
@@ -3000,7 +3663,7 @@
         <v>2.96946913717075</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B124">
         <v>39.513727286867699</v>
       </c>
@@ -3008,7 +3671,7 @@
         <v>1.4425054510387501</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B125">
         <v>21.7785202781028</v>
       </c>
@@ -3016,7 +3679,7 @@
         <v>0.66828161734851299</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B126">
         <v>11.524657179573101</v>
       </c>
@@ -3024,7 +3687,7 @@
         <v>0.29421098203768298</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B127">
         <v>5.8384040042946603</v>
       </c>
@@ -3032,7 +3695,7 @@
         <v>0.122595833264817</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B128">
         <v>2.8225209510382099</v>
       </c>
@@ -3040,7 +3703,7 @@
         <v>4.8132276540599997E-2</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B129">
         <v>1.29749453480608</v>
       </c>
@@ -3048,7 +3711,7 @@
         <v>1.7712542996566501E-2</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B130">
         <v>0</v>
       </c>

</xml_diff>